<commit_message>
rajout elements plan de test et bonus front-end
</commit_message>
<xml_diff>
--- a/P5_02_plantests.xlsx
+++ b/P5_02_plantests.xlsx
@@ -10,15 +10,14 @@
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Feuille 1'!$A$1:$F$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Feuille 1'!$A$1:$F$10</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -71,12 +70,6 @@
     </r>
   </si>
   <si>
-    <t>console.log() du résultat retourné par le serveur.</t>
-  </si>
-  <si>
-    <t>Problème de liaison au serveur car le serveur ne répond pas. (code erreur 500) ou erreur 400 (requête mal formulé côté client)</t>
-  </si>
-  <si>
     <t>La fonction doit retourner 'true' si l'input est rempli selon les critères de sa RegEx "'^[a-zA-Z0-9.-_]+[@]{1}[a-zA-Z0-9.-_]+[.]{1}[a-z]{2,10}$',
     "g" et 'false' si elle reçoit tout autre type de caractères ou nombres.</t>
   </si>
@@ -96,12 +89,6 @@
     <t>produit.js</t>
   </si>
   <si>
-    <t>12 à 21</t>
-  </si>
-  <si>
-    <t>La fonction doit servir à récupérer les Furnitures de l'API. Si tout se passe bien.</t>
-  </si>
-  <si>
     <t>Fetch(API/Furnitures)</t>
   </si>
   <si>
@@ -116,6 +103,93 @@
   <si>
     <t>On saisit le nom dans l'input (nom saisi selon les critères demandés), et on observe la valeur retournée, avec un console.log par exemple</t>
   </si>
+  <si>
+    <t>index.js</t>
+  </si>
+  <si>
+    <t>3 à 24</t>
+  </si>
+  <si>
+    <t>3 à 8</t>
+  </si>
+  <si>
+    <t>Problème de permission, de réseau, la fonction catch récupère l'erreur et l'affiche dans le console.log(erreur)</t>
+  </si>
+  <si>
+    <t>la deuxième fonction then(furnitures) doit récupérer tous les objets présents dans l'API</t>
+  </si>
+  <si>
+    <t>On fait un console.log(furnitures) et on vérifie dans la console si tous les objets du tableau ont été récupérés.</t>
+  </si>
+  <si>
+    <t>La première fonction then(response) nous permet de vérifier qu'on à bien une réponse, avant de pouvoir aller plus en avant et exploiter ce retour.</t>
+  </si>
+  <si>
+    <t>Fait un console,log(response) pour verifier la présence d'une reponse en json</t>
+  </si>
+  <si>
+    <t>Problème de permission, de réseau</t>
+  </si>
+  <si>
+    <t>Fetch(furniture/id)</t>
+  </si>
+  <si>
+    <t>Cette première fonction then(response) doit nous retourner une réponse qui correspond au produit choisi</t>
+  </si>
+  <si>
+    <t>On vérifie dans console.log(response) que l'id de l'objet sélectionné correspond bien à l'objet présent.</t>
+  </si>
+  <si>
+    <t>13 à 15</t>
+  </si>
+  <si>
+    <t>13 à 18</t>
+  </si>
+  <si>
+    <t>Cette deuxième fonction then(furniture) doit nous retourner les éléments de l'objet sélectionner</t>
+  </si>
+  <si>
+    <t>On vérifie dans console,log(furniture) que les  éléments présents, les options correspondent bien à l'objet sélectionné</t>
+  </si>
+  <si>
+    <t>Il peut y avoir un problème de réseau ou de permission, ou alors on peut avoir un mauvais id</t>
+  </si>
+  <si>
+    <t>Il peut y avoir des options qui manquent ou d'autres éléments de l'objet qui manquent</t>
+  </si>
+  <si>
+    <t>57 à 86</t>
+  </si>
+  <si>
+    <t>utils.js</t>
+  </si>
+  <si>
+    <t>8 à 19</t>
+  </si>
+  <si>
+    <t>function showQuantity()</t>
+  </si>
+  <si>
+    <t>cette fonction doit calculer le nombre d'article total envoyé au panier</t>
+  </si>
+  <si>
+    <t>la quantité totale d'articles ajoutés doit être présente sur le site web, à côté du panier</t>
+  </si>
+  <si>
+    <t>Cette fonction doit ajouter l'article sélectionné au panier</t>
+  </si>
+  <si>
+    <t>function ajouterArticle() 'condition panier vide'</t>
+  </si>
+  <si>
+    <t>On peut regarder dans la partie inspecteur/application de la page web si un article à bel et bien été ajouter dasn le localStorage</t>
+  </si>
+  <si>
+    <t>La somme calculée n'est pas exacte, erreur dans la formule de calcul, ou par exemple, si on ne fait pas un "parseInt" on aura une concaténation des chiffres au lieu d'avoir un calcul.</t>
+  </si>
+  <si>
+    <t>L'article peut être illisible dans le local storage si on ooublie de faire un JSON,stringify(panier) au moment de l'enoi dans le panier. A ce moment-là on aura un format [object ,object].</t>
+  </si>
 </sst>
 </file>
 
@@ -125,7 +199,7 @@
     <numFmt numFmtId="164" formatCode="[$-40C]General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +232,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,7 +297,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,7 +312,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -235,6 +321,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,17 +634,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:AMJ1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.19921875" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.09765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" style="2" customWidth="1"/>
     <col min="4" max="4" width="37.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="26.8984375" style="2" customWidth="1"/>
     <col min="6" max="6" width="31.59765625" style="2" customWidth="1"/>
@@ -593,122 +692,200 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:26" ht="52.8">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:26" ht="52.8">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="66">
+      <c r="A3" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="153" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="85.8" customHeight="1">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="B6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="C6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="66">
-      <c r="A4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="10" t="s">
+    </row>
+    <row r="7" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="153" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="76.5" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="B7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="66">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="66">
+      <c r="A9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="66">
+      <c r="A10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:26" ht="26.25" customHeight="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="26.25" customHeight="1">
@@ -731,7 +908,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="4:6" ht="26.25" customHeight="1">
+    <row r="17" spans="4:6" ht="25.5" customHeight="1">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -856,7 +1033,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="4:6" ht="25.5" customHeight="1">
+    <row r="42" spans="4:6" ht="13.8">
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -5626,20 +5803,15 @@
       <c r="E995" s="3"/>
       <c r="F995" s="3"/>
     </row>
-    <row r="996" spans="4:6" ht="13.8">
-      <c r="D996" s="3"/>
-      <c r="E996" s="3"/>
-      <c r="F996" s="3"/>
-    </row>
+    <row r="1048573" ht="12.75" customHeight="1"/>
     <row r="1048574" ht="12.75" customHeight="1"/>
     <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
-  <pageSetup paperSize="9" scale="84" fitToWidth="0" fitToHeight="0" orientation="landscape" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToWidth="0" fitToHeight="0" orientation="landscape" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="6" max="1048575" man="1"/>
+    <brk id="6" max="9" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>